<commit_message>
machineindex -> machineno 기준으로 변경 및 machineindex 컬럼 삭제. aging 기계도 machineindex: -1 -> machineno: 'aging'으로 변경
</commit_message>
<xml_diff>
--- a/python_engine/data/input/machine_master_info.xlsx
+++ b/python_engine/data/input/machine_master_info.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="machine_master" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,195 +436,154 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>machineindex</t>
+          <t>machineno</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>machineno</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>machinename</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A2020</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A2020</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>AgNW2호기</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C2010</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C2010</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>코팅1호기_WIN</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C2250</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C2250</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>코팅25호기_WIN</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C2260</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C2260</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>코팅26호기_WIN</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C2270</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C2270</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>코팅27호기_WIN</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>D2280</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>D2280</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>코팅28호기_DSP</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>O2310</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>O2310</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>코팅31호기_DSP</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>O2320</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>O2320</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>코팅32호기_DSP</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>O2340</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>O2340</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>코팅34호기_DSP</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>9</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>O2360</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>O2360</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
           <t>코팅36호기_DSP</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>O2510</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>O2510</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>코팅51호기(미사용)</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>11</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>O2590</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
-        <is>
-          <t>O2590</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
         <is>
           <t>코팅59호기_DSP</t>
         </is>

</xml_diff>